<commit_message>
add two correct cdot implementation python files
</commit_message>
<xml_diff>
--- a/source.xlsx
+++ b/source.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>1.56217</v>
+        <v>1.57672</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>1.50174</v>
+        <v>1.57672</v>
       </c>
     </row>
     <row r="18">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="20">
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="23">
@@ -611,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="24">
@@ -619,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="25">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="27">
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="28">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="29">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="30">
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="31">
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="32">
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="36">
@@ -715,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="37">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="38">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>1.85713</v>
+        <v>1.88589</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="42">
@@ -763,7 +763,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="43">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="44">
@@ -779,7 +779,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="45">
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="46">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="47">
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="48">
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="49">
@@ -819,7 +819,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="50">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="51">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="52">
@@ -843,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="53">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="54">
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="55">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>1.71592</v>
+        <v>1.64399</v>
       </c>
     </row>
     <row r="56">
@@ -875,7 +875,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="57">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="61">
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="62">
@@ -923,7 +923,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="63">
@@ -931,7 +931,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="64">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="65">
@@ -947,7 +947,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>1.90511</v>
+        <v>1.91194</v>
       </c>
     </row>
     <row r="66">
@@ -955,7 +955,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="67">
@@ -963,7 +963,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
     <row r="68">
@@ -971,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>1.50174</v>
+        <v>1.5278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
source data change from 005 to 030
</commit_message>
<xml_diff>
--- a/source.xlsx
+++ b/source.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.91194</v>
+        <v>1.90777</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.91194</v>
+        <v>1.80145</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.91194</v>
+        <v>1.78143</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.91194</v>
+        <v>1.72828</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.5278</v>
+        <v>1.66617</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.5278</v>
+        <v>1.51135</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1.91194</v>
+        <v>1.8809</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1.91194</v>
+        <v>1.8448</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1.91194</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1.91194</v>
+        <v>1.7384</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>1.57672</v>
+        <v>1.58262</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1.5278</v>
+        <v>1.58235</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1.91194</v>
+        <v>1.80395</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>1.91194</v>
+        <v>1.78267</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>1.91194</v>
+        <v>1.7603</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>1.57672</v>
+        <v>1.73087</v>
       </c>
     </row>
     <row r="18">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>1.5278</v>
+        <v>1.65433</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>1.91194</v>
+        <v>1.9052</v>
       </c>
     </row>
     <row r="20">
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>1.91194</v>
+        <v>1.76133</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>1.91194</v>
+        <v>1.73811</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>1.5278</v>
+        <v>1.77517</v>
       </c>
     </row>
     <row r="23">
@@ -611,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>1.5278</v>
+        <v>1.71755</v>
       </c>
     </row>
     <row r="24">
@@ -619,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>1.5278</v>
+        <v>1.66288</v>
       </c>
     </row>
     <row r="25">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>1.91194</v>
+        <v>1.81778</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>1.91194</v>
+        <v>1.78412</v>
       </c>
     </row>
     <row r="27">
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>1.5278</v>
+        <v>1.72424</v>
       </c>
     </row>
     <row r="28">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1.5278</v>
+        <v>1.73505</v>
       </c>
     </row>
     <row r="29">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>1.5278</v>
+        <v>1.53085</v>
       </c>
     </row>
     <row r="30">
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>1.91194</v>
+        <v>1.8972</v>
       </c>
     </row>
     <row r="31">
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>1.91194</v>
+        <v>1.78883</v>
       </c>
     </row>
     <row r="32">
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>1.5278</v>
+        <v>1.7591</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>1.5278</v>
+        <v>1.70897</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>1.5278</v>
+        <v>1.55268</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>1.5278</v>
+        <v>1.286</v>
       </c>
     </row>
     <row r="36">
@@ -715,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>1.91194</v>
+        <v>1.82057</v>
       </c>
     </row>
     <row r="37">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>1.91194</v>
+        <v>1.83973</v>
       </c>
     </row>
     <row r="38">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>1.91194</v>
+        <v>1.81615</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>1.88589</v>
+        <v>1.78485</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>1.5278</v>
+        <v>1.6856</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>1.5278</v>
+        <v>1.74728</v>
       </c>
     </row>
     <row r="42">
@@ -763,7 +763,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>1.91194</v>
+        <v>1.82195</v>
       </c>
     </row>
     <row r="43">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>1.91194</v>
+        <v>1.82747</v>
       </c>
     </row>
     <row r="44">
@@ -779,7 +779,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>1.5278</v>
+        <v>1.72439</v>
       </c>
     </row>
     <row r="45">
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>1.5278</v>
+        <v>1.69442</v>
       </c>
     </row>
     <row r="46">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>1.5278</v>
+        <v>1.7292</v>
       </c>
     </row>
     <row r="47">
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>1.91194</v>
+        <v>1.82863</v>
       </c>
     </row>
     <row r="48">
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>1.91194</v>
+        <v>1.8182</v>
       </c>
     </row>
     <row r="49">
@@ -819,7 +819,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>1.91194</v>
+        <v>1.77722</v>
       </c>
     </row>
     <row r="50">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>1.5278</v>
+        <v>1.7783</v>
       </c>
     </row>
     <row r="51">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>1.5278</v>
+        <v>1.67445</v>
       </c>
     </row>
     <row r="52">
@@ -843,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>1.5278</v>
+        <v>1.53795</v>
       </c>
     </row>
     <row r="53">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>1.91194</v>
+        <v>1.79462</v>
       </c>
     </row>
     <row r="54">
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>1.91194</v>
+        <v>1.8247</v>
       </c>
     </row>
     <row r="55">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>1.64399</v>
+        <v>1.7876</v>
       </c>
     </row>
     <row r="56">
@@ -875,7 +875,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>1.5278</v>
+        <v>1.6933</v>
       </c>
     </row>
     <row r="57">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>1.5278</v>
+        <v>1.70578</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>1.5278</v>
+        <v>1.58937</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>1.91194</v>
+        <v>1.79915</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>1.5278</v>
+        <v>1.78618</v>
       </c>
     </row>
     <row r="61">
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>1.5278</v>
+        <v>1.78602</v>
       </c>
     </row>
     <row r="62">
@@ -923,7 +923,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>1.5278</v>
+        <v>1.52465</v>
       </c>
     </row>
     <row r="63">
@@ -931,7 +931,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>1.5278</v>
+        <v>1.301</v>
       </c>
     </row>
     <row r="64">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>1.91194</v>
+        <v>1.8809</v>
       </c>
     </row>
     <row r="65">
@@ -947,7 +947,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>1.91194</v>
+        <v>1.6629</v>
       </c>
     </row>
     <row r="66">
@@ -955,7 +955,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>1.5278</v>
+        <v>1.7732</v>
       </c>
     </row>
     <row r="67">
@@ -963,7 +963,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>1.5278</v>
+        <v>1.58513</v>
       </c>
     </row>
     <row r="68">
@@ -971,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>1.5278</v>
+        <v>1.3856</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change derivation equation(gamma) and mapped source data(xt)
</commit_message>
<xml_diff>
--- a/source.xlsx
+++ b/source.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.90777</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.80145</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.78143</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.72828</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.66617</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.51135</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1.8809</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1.8448</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1.76</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1.7384</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>1.58262</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1.58235</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1.80395</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>1.78267</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>1.7603</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>1.73087</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="18">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>1.65433</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>1.9052</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="20">
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>1.76133</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>1.73811</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>1.77517</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="23">
@@ -611,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>1.71755</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="24">
@@ -619,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>1.66288</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="25">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>1.81778</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>1.78412</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="27">
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>1.72424</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="28">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1.73505</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="29">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>1.53085</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="30">
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>1.8972</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="31">
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>1.78883</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="32">
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>1.7591</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>1.70897</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>1.55268</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>1.286</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="36">
@@ -715,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>1.82057</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="37">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>1.83973</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="38">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>1.81615</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>1.78485</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>1.6856</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>1.74728</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="42">
@@ -763,7 +763,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>1.82195</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="43">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>1.82747</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="44">
@@ -779,7 +779,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>1.72439</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="45">
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>1.69442</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="46">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>1.7292</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="47">
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>1.82863</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="48">
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>1.8182</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="49">
@@ -819,7 +819,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>1.77722</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="50">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>1.7783</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="51">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>1.67445</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="52">
@@ -843,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>1.53795</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="53">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>1.79462</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="54">
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>1.8247</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="55">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>1.7876</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="56">
@@ -875,7 +875,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>1.6933</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="57">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>1.70578</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>1.58937</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>1.79915</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>1.78618</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="61">
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>1.78602</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="62">
@@ -923,7 +923,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>1.52465</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="63">
@@ -931,7 +931,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>1.301</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="64">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>1.8809</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="65">
@@ -947,7 +947,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>1.6629</v>
+        <v>1.78941</v>
       </c>
     </row>
     <row r="66">
@@ -955,7 +955,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>1.7732</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="67">
@@ -963,7 +963,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>1.58513</v>
+        <v>1.32543</v>
       </c>
     </row>
     <row r="68">
@@ -971,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>1.3856</v>
+        <v>1.32543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>